<commit_message>
Added visualizations and rearranged log output
</commit_message>
<xml_diff>
--- a/dyes_DFT_LDA_eth_dataset.xlsx
+++ b/dyes_DFT_LDA_eth_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,10 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>COSMO_Screening_Charge</t>
+          <t>Max_Absorption_nm</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Absorption_nm</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Max_f_osc</t>
         </is>
@@ -518,12 +513,9 @@
         <v>646.0990399999999</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>585</v>
       </c>
       <c r="J2" t="n">
-        <v>585</v>
-      </c>
-      <c r="K2" t="n">
         <v>0.9257919999999999</v>
       </c>
     </row>
@@ -555,12 +547,9 @@
         <v>832.68334</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>576</v>
       </c>
       <c r="J3" t="n">
-        <v>576</v>
-      </c>
-      <c r="K3" t="n">
         <v>0.898504</v>
       </c>
     </row>
@@ -592,12 +581,9 @@
         <v>761.7046810000001</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>938</v>
       </c>
       <c r="J4" t="n">
-        <v>938</v>
-      </c>
-      <c r="K4" t="n">
         <v>0.748518</v>
       </c>
     </row>
@@ -629,12 +615,9 @@
         <v>644.459413</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>934</v>
       </c>
       <c r="J5" t="n">
-        <v>934</v>
-      </c>
-      <c r="K5" t="n">
         <v>0.68387</v>
       </c>
     </row>
@@ -666,12 +649,9 @@
         <v>635.3120269999999</v>
       </c>
       <c r="I6" t="n">
-        <v>-0</v>
+        <v>918</v>
       </c>
       <c r="J6" t="n">
-        <v>918</v>
-      </c>
-      <c r="K6" t="n">
         <v>0.616428</v>
       </c>
     </row>
@@ -703,12 +683,9 @@
         <v>580.043959</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="J7" t="n">
-        <v>530</v>
-      </c>
-      <c r="K7" t="n">
         <v>0.912547</v>
       </c>
     </row>
@@ -740,12 +717,9 @@
         <v>659.6051</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>990</v>
       </c>
       <c r="J8" t="n">
-        <v>990</v>
-      </c>
-      <c r="K8" t="n">
         <v>0.598239</v>
       </c>
     </row>
@@ -777,12 +751,9 @@
         <v>738.046701</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>642</v>
       </c>
       <c r="J9" t="n">
-        <v>642</v>
-      </c>
-      <c r="K9" t="n">
         <v>0.6543369999999999</v>
       </c>
     </row>
@@ -814,12 +785,9 @@
         <v>819.062786</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>683</v>
       </c>
       <c r="J10" t="n">
-        <v>683</v>
-      </c>
-      <c r="K10" t="n">
         <v>1.467794</v>
       </c>
     </row>
@@ -851,12 +819,9 @@
         <v>405.588145</v>
       </c>
       <c r="I11" t="n">
-        <v>-0</v>
+        <v>415</v>
       </c>
       <c r="J11" t="n">
-        <v>415</v>
-      </c>
-      <c r="K11" t="n">
         <v>0.140013</v>
       </c>
     </row>
@@ -888,12 +853,9 @@
         <v>377.858553</v>
       </c>
       <c r="I12" t="n">
-        <v>-0</v>
+        <v>411</v>
       </c>
       <c r="J12" t="n">
-        <v>411</v>
-      </c>
-      <c r="K12" t="n">
         <v>0.262642</v>
       </c>
     </row>
@@ -925,12 +887,9 @@
         <v>395.333947</v>
       </c>
       <c r="I13" t="n">
-        <v>-0</v>
+        <v>358</v>
       </c>
       <c r="J13" t="n">
-        <v>358</v>
-      </c>
-      <c r="K13" t="n">
         <v>0.109675</v>
       </c>
     </row>
@@ -962,12 +921,9 @@
         <v>422.071911</v>
       </c>
       <c r="I14" t="n">
-        <v>-0</v>
+        <v>474</v>
       </c>
       <c r="J14" t="n">
-        <v>474</v>
-      </c>
-      <c r="K14" t="n">
         <v>0.498719</v>
       </c>
     </row>
@@ -999,12 +955,9 @@
         <v>447.552538</v>
       </c>
       <c r="I15" t="n">
-        <v>-0</v>
+        <v>519</v>
       </c>
       <c r="J15" t="n">
-        <v>519</v>
-      </c>
-      <c r="K15" t="n">
         <v>0.533673</v>
       </c>
     </row>
@@ -1036,12 +989,9 @@
         <v>345.067817</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="J16" t="n">
-        <v>342</v>
-      </c>
-      <c r="K16" t="n">
         <v>0.321588</v>
       </c>
     </row>
@@ -1073,12 +1023,9 @@
         <v>324.319271</v>
       </c>
       <c r="I17" t="n">
-        <v>-0</v>
+        <v>304</v>
       </c>
       <c r="J17" t="n">
-        <v>304</v>
-      </c>
-      <c r="K17" t="n">
         <v>0.321389</v>
       </c>
     </row>
@@ -1110,12 +1057,9 @@
         <v>322.019949</v>
       </c>
       <c r="I18" t="n">
-        <v>-0</v>
+        <v>328</v>
       </c>
       <c r="J18" t="n">
-        <v>328</v>
-      </c>
-      <c r="K18" t="n">
         <v>0.453893</v>
       </c>
     </row>
@@ -1147,12 +1091,9 @@
         <v>353.717532</v>
       </c>
       <c r="I19" t="n">
-        <v>-0</v>
+        <v>517</v>
       </c>
       <c r="J19" t="n">
-        <v>517</v>
-      </c>
-      <c r="K19" t="n">
         <v>0.55103</v>
       </c>
     </row>
@@ -1184,12 +1125,9 @@
         <v>417.187669</v>
       </c>
       <c r="I20" t="n">
-        <v>-0</v>
+        <v>273</v>
       </c>
       <c r="J20" t="n">
-        <v>273</v>
-      </c>
-      <c r="K20" t="n">
         <v>0.145043</v>
       </c>
     </row>
@@ -1221,12 +1159,9 @@
         <v>712.4113</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="J21" t="n">
-        <v>473</v>
-      </c>
-      <c r="K21" t="n">
         <v>0.379511</v>
       </c>
     </row>
@@ -1258,12 +1193,9 @@
         <v>383.364363</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>516</v>
       </c>
       <c r="J22" t="n">
-        <v>516</v>
-      </c>
-      <c r="K22" t="n">
         <v>0.948782</v>
       </c>
     </row>
@@ -1295,12 +1227,9 @@
         <v>432.277982</v>
       </c>
       <c r="I23" t="n">
-        <v>0</v>
+        <v>474</v>
       </c>
       <c r="J23" t="n">
-        <v>474</v>
-      </c>
-      <c r="K23" t="n">
         <v>0.708416</v>
       </c>
     </row>
@@ -1332,12 +1261,9 @@
         <v>410.949228</v>
       </c>
       <c r="I24" t="n">
-        <v>-0</v>
+        <v>552</v>
       </c>
       <c r="J24" t="n">
-        <v>552</v>
-      </c>
-      <c r="K24" t="n">
         <v>1.03911</v>
       </c>
     </row>
@@ -1369,12 +1295,9 @@
         <v>456.523894</v>
       </c>
       <c r="I25" t="n">
-        <v>-0</v>
+        <v>584</v>
       </c>
       <c r="J25" t="n">
-        <v>584</v>
-      </c>
-      <c r="K25" t="n">
         <v>0.695781</v>
       </c>
     </row>

</xml_diff>